<commit_message>
#Buat table generator           || Sudah #Isi table generator            || Sudah #Buat random number generator   || Sudah #Buat Fuzzification             || Sudah #Buat Inference                 || Sudah #Buat Defuzzification           || Belum
</commit_message>
<xml_diff>
--- a/Tugas_Kelompok_AI_Fuzzy/masukan.xlsx
+++ b/Tugas_Kelompok_AI_Fuzzy/masukan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="195">
   <si>
     <t>No</t>
   </si>
@@ -25,67 +25,580 @@
     <t>IPK</t>
   </si>
   <si>
-    <t>Gaji</t>
+    <t>Umur</t>
   </si>
   <si>
     <t>NXAZJ</t>
   </si>
   <si>
-    <t>3.08</t>
+    <t>0.51</t>
   </si>
   <si>
     <t>LGISN</t>
   </si>
   <si>
-    <t>0.72</t>
+    <t>2.44</t>
   </si>
   <si>
     <t>FLDNI</t>
   </si>
   <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>RUFTR</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>FLXXC</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>QXNSQ</t>
+  </si>
+  <si>
+    <t>1.57</t>
+  </si>
+  <si>
+    <t>FEGXC</t>
+  </si>
+  <si>
+    <t>2.73</t>
+  </si>
+  <si>
+    <t>GKKAO</t>
+  </si>
+  <si>
+    <t>1.61</t>
+  </si>
+  <si>
+    <t>KAQWX</t>
+  </si>
+  <si>
+    <t>2.59</t>
+  </si>
+  <si>
+    <t>NAAVF</t>
+  </si>
+  <si>
+    <t>2.91</t>
+  </si>
+  <si>
+    <t>YSFJD</t>
+  </si>
+  <si>
+    <t>3.24</t>
+  </si>
+  <si>
+    <t>UNDVS</t>
+  </si>
+  <si>
+    <t>2.28</t>
+  </si>
+  <si>
+    <t>FXMHQ</t>
+  </si>
+  <si>
+    <t>3.96</t>
+  </si>
+  <si>
+    <t>TWKZB</t>
+  </si>
+  <si>
+    <t>2.01</t>
+  </si>
+  <si>
+    <t>HDPGX</t>
+  </si>
+  <si>
+    <t>2.15</t>
+  </si>
+  <si>
+    <t>ZYRVF</t>
+  </si>
+  <si>
+    <t>2.63</t>
+  </si>
+  <si>
+    <t>ISNQE</t>
+  </si>
+  <si>
+    <t>3.89</t>
+  </si>
+  <si>
+    <t>BFJAE</t>
+  </si>
+  <si>
+    <t>2.81</t>
+  </si>
+  <si>
+    <t>HLRKF</t>
+  </si>
+  <si>
+    <t>3.67</t>
+  </si>
+  <si>
+    <t>MKABB</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>WOCMZ</t>
+  </si>
+  <si>
+    <t>1.69</t>
+  </si>
+  <si>
+    <t>FZAYW</t>
+  </si>
+  <si>
+    <t>LGVQY</t>
+  </si>
+  <si>
+    <t>2.93</t>
+  </si>
+  <si>
+    <t>DPTBA</t>
+  </si>
+  <si>
+    <t>3.32</t>
+  </si>
+  <si>
+    <t>UPKYT</t>
+  </si>
+  <si>
+    <t>1.07</t>
+  </si>
+  <si>
+    <t>NRGLY</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>VWDRE</t>
+  </si>
+  <si>
+    <t>1.65</t>
+  </si>
+  <si>
+    <t>CPFKH</t>
+  </si>
+  <si>
+    <t>GFFJE</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>RCQWA</t>
+  </si>
+  <si>
+    <t>1.56</t>
+  </si>
+  <si>
+    <t>EAVPF</t>
+  </si>
+  <si>
+    <t>2.57</t>
+  </si>
+  <si>
+    <t>TZDIQ</t>
+  </si>
+  <si>
+    <t>2.96</t>
+  </si>
+  <si>
+    <t>YMCZY</t>
+  </si>
+  <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>ONFHF</t>
+  </si>
+  <si>
+    <t>2.48</t>
+  </si>
+  <si>
+    <t>ALKFM</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>FFSVQ</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>HNQWN</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>KDCUO</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>XGUTS</t>
+  </si>
+  <si>
+    <t>2.72</t>
+  </si>
+  <si>
+    <t>GXEQH</t>
+  </si>
+  <si>
+    <t>3.65</t>
+  </si>
+  <si>
+    <t>KSJER</t>
+  </si>
+  <si>
+    <t>1.55</t>
+  </si>
+  <si>
+    <t>QWYVZ</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>BIYNB</t>
+  </si>
+  <si>
+    <t>2.51</t>
+  </si>
+  <si>
+    <t>LZQRS</t>
+  </si>
+  <si>
+    <t>DUYCE</t>
+  </si>
+  <si>
+    <t>0.16</t>
+  </si>
+  <si>
+    <t>LWUBI</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>XOVLM</t>
+  </si>
+  <si>
+    <t>2.40</t>
+  </si>
+  <si>
+    <t>JOTIJ</t>
+  </si>
+  <si>
+    <t>1.83</t>
+  </si>
+  <si>
+    <t>XPPBI</t>
+  </si>
+  <si>
+    <t>1.39</t>
+  </si>
+  <si>
+    <t>OAHLE</t>
+  </si>
+  <si>
+    <t>AVUZC</t>
+  </si>
+  <si>
+    <t>0.55</t>
+  </si>
+  <si>
+    <t>ADTGM</t>
+  </si>
+  <si>
+    <t>3.07</t>
+  </si>
+  <si>
+    <t>PFILG</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>JXKMC</t>
+  </si>
+  <si>
+    <t>2.76</t>
+  </si>
+  <si>
+    <t>TJLZB</t>
+  </si>
+  <si>
+    <t>2.27</t>
+  </si>
+  <si>
+    <t>NGFCE</t>
+  </si>
+  <si>
+    <t>3.60</t>
+  </si>
+  <si>
+    <t>JHKNG</t>
+  </si>
+  <si>
+    <t>3.19</t>
+  </si>
+  <si>
+    <t>AEDQB</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>ZKMKB</t>
+  </si>
+  <si>
+    <t>1.81</t>
+  </si>
+  <si>
+    <t>HDPES</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>GISRL</t>
+  </si>
+  <si>
+    <t>3.02</t>
+  </si>
+  <si>
+    <t>FXJBC</t>
+  </si>
+  <si>
+    <t>DQGRQ</t>
+  </si>
+  <si>
+    <t>3.91</t>
+  </si>
+  <si>
+    <t>VNQAY</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>QESRK</t>
+  </si>
+  <si>
+    <t>2.03</t>
+  </si>
+  <si>
+    <t>SYZFO</t>
+  </si>
+  <si>
+    <t>1.97</t>
+  </si>
+  <si>
+    <t>NOALV</t>
+  </si>
+  <si>
+    <t>3.31</t>
+  </si>
+  <si>
+    <t>AMLVR</t>
+  </si>
+  <si>
+    <t>2.38</t>
+  </si>
+  <si>
+    <t>VTAKP</t>
+  </si>
+  <si>
+    <t>3.52</t>
+  </si>
+  <si>
+    <t>OBKKM</t>
+  </si>
+  <si>
+    <t>1.28</t>
+  </si>
+  <si>
+    <t>ZJEMS</t>
+  </si>
+  <si>
+    <t>0.39</t>
+  </si>
+  <si>
+    <t>TBSDP</t>
+  </si>
+  <si>
+    <t>0.74</t>
+  </si>
+  <si>
+    <t>DDTFB</t>
+  </si>
+  <si>
+    <t>0.19</t>
+  </si>
+  <si>
+    <t>BJGQD</t>
+  </si>
+  <si>
+    <t>2.83</t>
+  </si>
+  <si>
+    <t>OPPBN</t>
+  </si>
+  <si>
+    <t>2.74</t>
+  </si>
+  <si>
+    <t>HHKXZ</t>
+  </si>
+  <si>
+    <t>FMSRH</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>VPFGR</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>SRUGF</t>
+  </si>
+  <si>
+    <t>0.26</t>
+  </si>
+  <si>
+    <t>VXOYA</t>
+  </si>
+  <si>
+    <t>2.64</t>
+  </si>
+  <si>
+    <t>UGCZY</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>CRZDD</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>ISHGI</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t>HPLXW</t>
+  </si>
+  <si>
+    <t>2.61</t>
+  </si>
+  <si>
+    <t>OVMRH</t>
+  </si>
+  <si>
+    <t>2.46</t>
+  </si>
+  <si>
+    <t>UOQDQ</t>
+  </si>
+  <si>
+    <t>3.80</t>
+  </si>
+  <si>
+    <t>AQRVL</t>
+  </si>
+  <si>
+    <t>3.90</t>
+  </si>
+  <si>
+    <t>HMPVC</t>
+  </si>
+  <si>
+    <t>1.24</t>
+  </si>
+  <si>
+    <t>NODKH</t>
+  </si>
+  <si>
+    <t>OJNSD</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>FGXTM</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>ISUYZ</t>
+  </si>
+  <si>
+    <t>1.75</t>
+  </si>
+  <si>
+    <t>FUAQX</t>
+  </si>
+  <si>
+    <t>XIAZP</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>KWUGZ</t>
+  </si>
+  <si>
     <t>0.40</t>
   </si>
   <si>
-    <t>RUFTR</t>
-  </si>
-  <si>
-    <t>1.66</t>
-  </si>
-  <si>
-    <t>FLXXC</t>
-  </si>
-  <si>
-    <t>3.54</t>
-  </si>
-  <si>
-    <t>QXNSQ</t>
-  </si>
-  <si>
-    <t>2.31</t>
-  </si>
-  <si>
-    <t>FEGXC</t>
-  </si>
-  <si>
-    <t>2.95</t>
-  </si>
-  <si>
-    <t>GKKAO</t>
-  </si>
-  <si>
-    <t>0.93</t>
-  </si>
-  <si>
-    <t>KAQWX</t>
-  </si>
-  <si>
-    <t>2.09</t>
-  </si>
-  <si>
-    <t>NAAVF</t>
-  </si>
-  <si>
-    <t>2.84</t>
+    <t>UJAXM</t>
+  </si>
+  <si>
+    <t>LGRIH</t>
+  </si>
+  <si>
+    <t>2.69</t>
+  </si>
+  <si>
+    <t>CZGIR</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>AAESS</t>
+  </si>
+  <si>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>ZZEKG</t>
+  </si>
+  <si>
+    <t>0.79</t>
   </si>
 </sst>
 </file>
@@ -417,7 +930,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -462,7 +975,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -476,7 +989,7 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -490,7 +1003,7 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -504,7 +1017,7 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -518,7 +1031,7 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -532,7 +1045,7 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -546,7 +1059,7 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -560,7 +1073,7 @@
         <v>21</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -574,6 +1087,1266 @@
         <v>23</v>
       </c>
       <c r="D11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" t="s">
+        <v>121</v>
+      </c>
+      <c r="D62">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>123</v>
+      </c>
+      <c r="C64" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>125</v>
+      </c>
+      <c r="C65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" t="s">
+        <v>130</v>
+      </c>
+      <c r="D67">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" t="s">
+        <v>140</v>
+      </c>
+      <c r="D72">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>141</v>
+      </c>
+      <c r="C73" t="s">
+        <v>142</v>
+      </c>
+      <c r="D73">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" t="s">
+        <v>144</v>
+      </c>
+      <c r="D74">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>145</v>
+      </c>
+      <c r="C75" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>147</v>
+      </c>
+      <c r="C76" t="s">
+        <v>148</v>
+      </c>
+      <c r="D76">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>149</v>
+      </c>
+      <c r="C77" t="s">
+        <v>121</v>
+      </c>
+      <c r="D77">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" t="s">
+        <v>151</v>
+      </c>
+      <c r="D78">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" t="s">
+        <v>153</v>
+      </c>
+      <c r="D79">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" t="s">
+        <v>155</v>
+      </c>
+      <c r="D80">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>156</v>
+      </c>
+      <c r="C81" t="s">
+        <v>157</v>
+      </c>
+      <c r="D81">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" t="s">
+        <v>159</v>
+      </c>
+      <c r="D82">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" t="s">
+        <v>163</v>
+      </c>
+      <c r="D84">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>164</v>
+      </c>
+      <c r="C85" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>166</v>
+      </c>
+      <c r="C86" t="s">
+        <v>167</v>
+      </c>
+      <c r="D86">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>168</v>
+      </c>
+      <c r="C87" t="s">
+        <v>169</v>
+      </c>
+      <c r="D87">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>170</v>
+      </c>
+      <c r="C88" t="s">
+        <v>171</v>
+      </c>
+      <c r="D88">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>172</v>
+      </c>
+      <c r="C89" t="s">
+        <v>173</v>
+      </c>
+      <c r="D89">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>174</v>
+      </c>
+      <c r="C90" t="s">
+        <v>54</v>
+      </c>
+      <c r="D90">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>175</v>
+      </c>
+      <c r="C91" t="s">
+        <v>176</v>
+      </c>
+      <c r="D91">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>177</v>
+      </c>
+      <c r="C92" t="s">
+        <v>178</v>
+      </c>
+      <c r="D92">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>179</v>
+      </c>
+      <c r="C93" t="s">
+        <v>180</v>
+      </c>
+      <c r="D93">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>181</v>
+      </c>
+      <c r="C94" t="s">
+        <v>63</v>
+      </c>
+      <c r="D94">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>182</v>
+      </c>
+      <c r="C95" t="s">
+        <v>183</v>
+      </c>
+      <c r="D95">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>184</v>
+      </c>
+      <c r="C96" t="s">
+        <v>185</v>
+      </c>
+      <c r="D96">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" t="s">
+        <v>148</v>
+      </c>
+      <c r="D97">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>187</v>
+      </c>
+      <c r="C98" t="s">
+        <v>188</v>
+      </c>
+      <c r="D98">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>189</v>
+      </c>
+      <c r="C99" t="s">
+        <v>190</v>
+      </c>
+      <c r="D99">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>191</v>
+      </c>
+      <c r="C100" t="s">
+        <v>192</v>
+      </c>
+      <c r="D100">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>193</v>
+      </c>
+      <c r="C101" t="s">
+        <v>194</v>
+      </c>
+      <c r="D101">
         <v>19</v>
       </c>
     </row>

</xml_diff>